<commit_message>
Implemented and passed all test cases
</commit_message>
<xml_diff>
--- a/Documentatie/Test_cases.xlsx
+++ b/Documentatie/Test_cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivier\Documents\Fontys\Semester 2\Individueel traject\Ontwikkelopdracht\RaadHetWoordAsp\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341A96AE-9AC2-46EF-A16F-D29C8B6B8A13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7884B5F4-59A6-4FE4-9F20-4680D6A4A3D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{FFF3AB20-DF7B-4820-8C3A-4A4ADF34EE9B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
   <si>
     <t>Testcases</t>
   </si>
@@ -343,13 +343,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF4E6F1-32CA-4564-BE24-7F11FBD6944A}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +741,16 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -749,7 +758,7 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -764,7 +773,16 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -772,7 +790,7 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -787,7 +805,16 @@
       <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -795,7 +822,7 @@
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="9"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -810,13 +837,22 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="F11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -831,13 +867,22 @@
       <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="F13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
-      <c r="K14" s="9"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -852,6 +897,15 @@
       <c r="D16" t="s">
         <v>33</v>
       </c>
+      <c r="F16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K16" s="5" t="s">
         <v>21</v>
       </c>
@@ -869,6 +923,15 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K17" s="5" t="s">
         <v>21</v>
       </c>
@@ -886,6 +949,15 @@
       <c r="D19" t="s">
         <v>39</v>
       </c>
+      <c r="F19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K19" s="5" t="s">
         <v>21</v>
       </c>
@@ -903,6 +975,15 @@
       <c r="D20" t="s">
         <v>40</v>
       </c>
+      <c r="F20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K20" s="5" t="s">
         <v>21</v>
       </c>
@@ -920,6 +1001,15 @@
       <c r="D21" t="s">
         <v>43</v>
       </c>
+      <c r="F21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K21" s="5" t="s">
         <v>21</v>
       </c>
@@ -937,6 +1027,15 @@
       <c r="D23" t="s">
         <v>59</v>
       </c>
+      <c r="F23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K23" s="5" t="s">
         <v>21</v>
       </c>
@@ -954,6 +1053,15 @@
       <c r="D24" t="s">
         <v>60</v>
       </c>
+      <c r="F24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K24" s="5" t="s">
         <v>21</v>
       </c>
@@ -971,6 +1079,15 @@
       <c r="D26" t="s">
         <v>57</v>
       </c>
+      <c r="F26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K26" s="5" t="s">
         <v>21</v>
       </c>
@@ -988,6 +1105,15 @@
       <c r="D27" t="s">
         <v>56</v>
       </c>
+      <c r="F27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="K27" s="5" t="s">
         <v>21</v>
       </c>
@@ -1002,16 +1128,25 @@
       <c r="C29" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="F29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="8"/>
-      <c r="K30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -1023,18 +1158,27 @@
       <c r="C31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="F31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="7"/>
-      <c r="K32" s="9"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -1047,8 +1191,20 @@
       <c r="D34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>75</v>
       </c>
@@ -1061,8 +1217,20 @@
       <c r="D35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>76</v>
       </c>
@@ -1075,20 +1243,32 @@
       <c r="D37" t="s">
         <v>79</v>
       </c>
+      <c r="F37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="K13:K14"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="K29:K30"/>
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C13:C14"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K13:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>